<commit_message>
Adding sample file for Employess
</commit_message>
<xml_diff>
--- a/ReSources/AllEmployee.xlsx
+++ b/ReSources/AllEmployee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AaWork\Amezon\ReSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZLearning\KC\ReSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0C403-8A2C-49BC-819D-5AA4D4BA7D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34DA083-A2D4-4D97-BF2D-873286E8AA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{65C14963-D7D9-489F-85DF-B390E3AF6B64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{65C14963-D7D9-489F-85DF-B390E3AF6B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -6944,24 +6944,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E260FD4-E818-43DD-82F8-08E3A45897CD}">
   <dimension ref="A1:L1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
@@ -7572,7 +7572,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="13.8" customHeight="1">
       <c r="A17" t="s">
         <v>147</v>
       </c>
@@ -45023,15 +45023,15 @@
       <selection activeCell="C18" activeCellId="1" sqref="C15 C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" customWidth="1"/>
-    <col min="9" max="9" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">

</xml_diff>